<commit_message>
We tesd only males, females, special needs and grades. We need more dynamic characteristics
</commit_message>
<xml_diff>
--- a/new_students.xlsx
+++ b/new_students.xlsx
@@ -13273,7 +13273,7 @@
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
@@ -13345,7 +13345,7 @@
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R3" t="n">
         <v>1</v>
@@ -13417,7 +13417,7 @@
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
         <v>2</v>
@@ -13491,7 +13491,7 @@
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R5" t="n">
         <v>3</v>
@@ -13637,7 +13637,7 @@
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" t="n">
         <v>5</v>
@@ -13709,7 +13709,7 @@
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R8" t="n">
         <v>6</v>
@@ -13783,7 +13783,7 @@
       </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R9" t="n">
         <v>7</v>
@@ -13855,7 +13855,7 @@
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" t="n">
         <v>8</v>
@@ -14001,7 +14001,7 @@
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R12" t="n">
         <v>10</v>
@@ -14073,7 +14073,7 @@
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R13" t="n">
         <v>11</v>
@@ -14145,7 +14145,7 @@
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R14" t="n">
         <v>12</v>
@@ -14219,7 +14219,7 @@
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R15" t="n">
         <v>13</v>
@@ -14291,7 +14291,7 @@
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R16" t="n">
         <v>14</v>
@@ -14511,7 +14511,7 @@
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R19" t="n">
         <v>17</v>
@@ -14657,7 +14657,7 @@
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R21" t="n">
         <v>19</v>
@@ -14803,7 +14803,7 @@
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R23" t="n">
         <v>21</v>
@@ -14877,7 +14877,7 @@
       </c>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R24" t="n">
         <v>22</v>
@@ -14949,7 +14949,7 @@
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25" t="n">
         <v>23</v>
@@ -15021,7 +15021,7 @@
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R26" t="n">
         <v>24</v>
@@ -15165,7 +15165,7 @@
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R28" t="n">
         <v>26</v>
@@ -15237,7 +15237,7 @@
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R29" t="n">
         <v>27</v>
@@ -15309,7 +15309,7 @@
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R30" t="n">
         <v>28</v>
@@ -15381,7 +15381,7 @@
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R31" t="n">
         <v>29</v>
@@ -15527,7 +15527,7 @@
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R33" t="n">
         <v>31</v>
@@ -15601,7 +15601,7 @@
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R34" t="n">
         <v>14</v>
@@ -15675,7 +15675,7 @@
       </c>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R35" t="n">
         <v>32</v>
@@ -15749,7 +15749,7 @@
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R36" t="n">
         <v>23</v>
@@ -15825,7 +15825,7 @@
       </c>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R37" t="n">
         <v>33</v>
@@ -15897,7 +15897,7 @@
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R38" t="n">
         <v>34</v>
@@ -15969,7 +15969,7 @@
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R39" t="n">
         <v>35</v>
@@ -16045,7 +16045,7 @@
       </c>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R40" t="n">
         <v>36</v>
@@ -16117,7 +16117,7 @@
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R41" t="n">
         <v>37</v>
@@ -16189,7 +16189,7 @@
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R42" t="n">
         <v>36</v>
@@ -16261,7 +16261,7 @@
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R43" t="n">
         <v>38</v>
@@ -16333,7 +16333,7 @@
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R44" t="n">
         <v>39</v>
@@ -16407,7 +16407,7 @@
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R45" t="n">
         <v>0</v>
@@ -16479,7 +16479,7 @@
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46" t="n">
         <v>40</v>
@@ -16551,7 +16551,7 @@
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R47" t="n">
         <v>41</v>
@@ -16839,7 +16839,7 @@
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R51" t="n">
         <v>31</v>
@@ -16913,7 +16913,7 @@
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R52" t="n">
         <v>45</v>
@@ -16985,7 +16985,7 @@
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R53" t="n">
         <v>45</v>
@@ -17059,7 +17059,7 @@
       </c>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R54" t="n">
         <v>19</v>
@@ -17133,7 +17133,7 @@
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R55" t="n">
         <v>41</v>
@@ -17207,7 +17207,7 @@
       </c>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R56" t="n">
         <v>46</v>
@@ -17279,7 +17279,7 @@
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R57" t="n">
         <v>47</v>
@@ -17353,7 +17353,7 @@
       </c>
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R58" t="n">
         <v>48</v>
@@ -17425,7 +17425,7 @@
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R59" t="n">
         <v>49</v>
@@ -17571,7 +17571,7 @@
       <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R61" t="n">
         <v>23</v>
@@ -17645,7 +17645,7 @@
       </c>
       <c r="P62" t="inlineStr"/>
       <c r="Q62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R62" t="n">
         <v>51</v>
@@ -17717,7 +17717,7 @@
       <c r="O63" t="inlineStr"/>
       <c r="P63" t="inlineStr"/>
       <c r="Q63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R63" t="n">
         <v>52</v>
@@ -17789,7 +17789,7 @@
       <c r="O64" t="inlineStr"/>
       <c r="P64" t="inlineStr"/>
       <c r="Q64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R64" t="n">
         <v>13</v>
@@ -17935,7 +17935,7 @@
       <c r="O66" t="inlineStr"/>
       <c r="P66" t="inlineStr"/>
       <c r="Q66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R66" t="n">
         <v>39</v>
@@ -18153,7 +18153,7 @@
       <c r="O69" t="inlineStr"/>
       <c r="P69" t="inlineStr"/>
       <c r="Q69" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R69" t="n">
         <v>54</v>
@@ -18227,7 +18227,7 @@
       <c r="O70" t="inlineStr"/>
       <c r="P70" t="inlineStr"/>
       <c r="Q70" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R70" t="n">
         <v>49</v>
@@ -18299,7 +18299,7 @@
       <c r="O71" t="inlineStr"/>
       <c r="P71" t="inlineStr"/>
       <c r="Q71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R71" t="n">
         <v>55</v>
@@ -18443,7 +18443,7 @@
       <c r="O73" t="inlineStr"/>
       <c r="P73" t="inlineStr"/>
       <c r="Q73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R73" t="n">
         <v>3</v>
@@ -18515,7 +18515,7 @@
       <c r="O74" t="inlineStr"/>
       <c r="P74" t="inlineStr"/>
       <c r="Q74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R74" t="n">
         <v>33</v>
@@ -18589,7 +18589,7 @@
       <c r="O75" t="inlineStr"/>
       <c r="P75" t="inlineStr"/>
       <c r="Q75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R75" t="n">
         <v>8</v>
@@ -18733,7 +18733,7 @@
       <c r="O77" t="inlineStr"/>
       <c r="P77" t="inlineStr"/>
       <c r="Q77" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R77" t="n">
         <v>57</v>
@@ -18881,7 +18881,7 @@
       </c>
       <c r="P79" t="inlineStr"/>
       <c r="Q79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R79" t="n">
         <v>59</v>
@@ -18955,7 +18955,7 @@
       </c>
       <c r="P80" t="inlineStr"/>
       <c r="Q80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R80" t="n">
         <v>60</v>
@@ -19029,7 +19029,7 @@
       <c r="O81" t="inlineStr"/>
       <c r="P81" t="inlineStr"/>
       <c r="Q81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R81" t="n">
         <v>61</v>
@@ -19101,7 +19101,7 @@
       <c r="O82" t="inlineStr"/>
       <c r="P82" t="inlineStr"/>
       <c r="Q82" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R82" t="n">
         <v>62</v>
@@ -19249,7 +19249,7 @@
       </c>
       <c r="P84" t="inlineStr"/>
       <c r="Q84" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R84" t="n">
         <v>64</v>
@@ -19469,7 +19469,7 @@
       </c>
       <c r="P87" t="inlineStr"/>
       <c r="Q87" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R87" t="n">
         <v>66</v>
@@ -19541,7 +19541,7 @@
       <c r="O88" t="inlineStr"/>
       <c r="P88" t="inlineStr"/>
       <c r="Q88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R88" t="n">
         <v>67</v>
@@ -19615,7 +19615,7 @@
       <c r="O89" t="inlineStr"/>
       <c r="P89" t="inlineStr"/>
       <c r="Q89" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R89" t="n">
         <v>21</v>
@@ -19691,7 +19691,7 @@
       </c>
       <c r="P90" t="inlineStr"/>
       <c r="Q90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R90" t="n">
         <v>14</v>
@@ -19765,7 +19765,7 @@
       <c r="O91" t="inlineStr"/>
       <c r="P91" t="inlineStr"/>
       <c r="Q91" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R91" t="n">
         <v>55</v>
@@ -19839,7 +19839,7 @@
       <c r="O92" t="inlineStr"/>
       <c r="P92" t="inlineStr"/>
       <c r="Q92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R92" t="n">
         <v>31</v>
@@ -19911,7 +19911,7 @@
       <c r="O93" t="inlineStr"/>
       <c r="P93" t="inlineStr"/>
       <c r="Q93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R93" t="n">
         <v>68</v>
@@ -19983,7 +19983,7 @@
       <c r="O94" t="inlineStr"/>
       <c r="P94" t="inlineStr"/>
       <c r="Q94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R94" t="n">
         <v>61</v>
@@ -20057,7 +20057,7 @@
       </c>
       <c r="P95" t="inlineStr"/>
       <c r="Q95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R95" t="n">
         <v>69</v>
@@ -20201,7 +20201,7 @@
       <c r="O97" t="inlineStr"/>
       <c r="P97" t="inlineStr"/>
       <c r="Q97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R97" t="n">
         <v>71</v>
@@ -20349,7 +20349,7 @@
       <c r="O99" t="inlineStr"/>
       <c r="P99" t="inlineStr"/>
       <c r="Q99" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R99" t="n">
         <v>21</v>
@@ -20421,7 +20421,7 @@
       <c r="O100" t="inlineStr"/>
       <c r="P100" t="inlineStr"/>
       <c r="Q100" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R100" t="n">
         <v>72</v>

</xml_diff>